<commit_message>
Aumento probabilidad generacion plataformas rojas
</commit_message>
<xml_diff>
--- a/Probabilidades objetos.xlsx
+++ b/Probabilidades objetos.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Dropbox\Ingenieria del Sotfware\Tercero\2º Semestre\(Optativa) Diseño y Programación de Videojuegos\Juego Doodle Jump Unity\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B93A324-847F-4FB1-AC33-1E40B919B7E5}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0F13F91-8E3A-4B7D-BE47-D1AEFC971115}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28770" windowHeight="12135" xr2:uid="{034BC0E4-55F9-4994-93FB-DB6BF41EED07}"/>
   </bookViews>
@@ -30,6 +30,24 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={B4728D91-734D-45EC-A2E1-D62CEE5C7A47}</author>
+  </authors>
+  <commentList>
+    <comment ref="C5" authorId="0" shapeId="0" xr:uid="{B4728D91-734D-45EC-A2E1-D62CEE5C7A47}">
+      <text>
+        <t>[Comentario encadenado]
+Su versión de Excel le permite leer este comentario encadenado; sin embargo, las ediciones que se apliquen se quitarán si el archivo se abre en una versión más reciente de Excel. Más información: https://go.microsoft.com/fwlink/?linkid=870924
+Comentario:
+    Aumentada por código para que se generen más rojas</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
@@ -103,13 +121,19 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -151,6 +175,12 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <person displayName="Alvaro" id="{7BF96F9D-0C38-41AC-9956-524D0F4191CF}" userId="Alvaro" providerId="None"/>
+</personList>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -448,12 +478,20 @@
 </a:theme>
 </file>
 
+<file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="C5" dT="2019-01-13T13:07:04.82" personId="{7BF96F9D-0C38-41AC-9956-524D0F4191CF}" id="{B4728D91-734D-45EC-A2E1-D62CEE5C7A47}">
+    <text>Aumentada por código para que se generen más rojas</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12023AB2-F6EA-4BFB-8062-39FB411D6EED}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12023AB2-F6EA-4BFB-8062-39FB411D6EED}">
   <dimension ref="B3:E14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K24" sqref="K24"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -598,5 +636,6 @@
     <ignoredError sqref="E3" twoDigitTextYear="1"/>
     <ignoredError sqref="E13" numberStoredAsText="1"/>
   </ignoredErrors>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Cambio probabilidades generacion elementos
</commit_message>
<xml_diff>
--- a/Probabilidades objetos.xlsx
+++ b/Probabilidades objetos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Dropbox\Ingenieria del Sotfware\Tercero\2º Semestre\(Optativa) Diseño y Programación de Videojuegos\Juego Doodle Jump Unity\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0F13F91-8E3A-4B7D-BE47-D1AEFC971115}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12841244-8211-48A5-B91B-471A343D3D78}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28770" windowHeight="12135" xr2:uid="{034BC0E4-55F9-4994-93FB-DB6BF41EED07}"/>
   </bookViews>
@@ -84,37 +84,37 @@
     <t>enemigoVerde</t>
   </si>
   <si>
-    <t>1-45</t>
-  </si>
-  <si>
-    <t>46-55</t>
-  </si>
-  <si>
-    <t>56-65</t>
-  </si>
-  <si>
-    <t>66-71</t>
-  </si>
-  <si>
-    <t>72-81</t>
-  </si>
-  <si>
-    <t>82-86</t>
-  </si>
-  <si>
-    <t>87-90</t>
-  </si>
-  <si>
-    <t>91-94</t>
-  </si>
-  <si>
     <t>95-97</t>
   </si>
   <si>
-    <t>98-99</t>
-  </si>
-  <si>
-    <t>100</t>
+    <t>1-44</t>
+  </si>
+  <si>
+    <t>98-100</t>
+  </si>
+  <si>
+    <t>45-54</t>
+  </si>
+  <si>
+    <t>55-62</t>
+  </si>
+  <si>
+    <t>63-68</t>
+  </si>
+  <si>
+    <t>69-78</t>
+  </si>
+  <si>
+    <t>79-83</t>
+  </si>
+  <si>
+    <t>84-87</t>
+  </si>
+  <si>
+    <t>88-91</t>
+  </si>
+  <si>
+    <t>92-94</t>
   </si>
 </sst>
 </file>
@@ -491,7 +491,7 @@
   <dimension ref="B3:E14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -507,10 +507,10 @@
         <v>0</v>
       </c>
       <c r="C3" s="1">
-        <v>0.45</v>
+        <v>0.44</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.25">
@@ -521,7 +521,7 @@
         <v>0.1</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.25">
@@ -529,10 +529,10 @@
         <v>3</v>
       </c>
       <c r="C5" s="1">
-        <v>0.1</v>
+        <v>0.08</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.25">
@@ -543,7 +543,7 @@
         <v>0.06</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.25">
@@ -554,7 +554,7 @@
         <v>0.1</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.25">
@@ -565,7 +565,7 @@
         <v>0.05</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.25">
@@ -576,7 +576,7 @@
         <v>0.04</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.25">
@@ -587,7 +587,7 @@
         <v>0.04</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.25">
@@ -598,7 +598,7 @@
         <v>0.03</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.25">
@@ -606,10 +606,10 @@
         <v>9</v>
       </c>
       <c r="C12" s="1">
-        <v>0.02</v>
+        <v>0.03</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.25">
@@ -617,10 +617,10 @@
         <v>10</v>
       </c>
       <c r="C13" s="1">
-        <v>0.01</v>
+        <v>0.03</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
     </row>
     <row r="14" spans="2:5" x14ac:dyDescent="0.25">
@@ -634,7 +634,6 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
     <ignoredError sqref="E3" twoDigitTextYear="1"/>
-    <ignoredError sqref="E13" numberStoredAsText="1"/>
   </ignoredErrors>
   <legacyDrawing r:id="rId2"/>
 </worksheet>

</xml_diff>